<commit_message>
feat: add tahun_ajar_id into kelas for alumni feature, and fix some bug when add the id
</commit_message>
<xml_diff>
--- a/public/assets/import/contoh_format_import_kelas.xlsx
+++ b/public/assets/import/contoh_format_import_kelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1zaru\Downloads\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ngoding\sipapii\public\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF9B2E5-168D-4A4D-AFEA-212A108B79A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A70E4F0-C293-4A49-8F09-C7D75CDE1D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34680" yWindow="3975" windowWidth="17280" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36525" yWindow="2670" windowWidth="13830" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>